<commit_message>
reconciled subjects and prepared OLR for test ingest
</commit_message>
<xml_diff>
--- a/keeling/OLR/OLR_keeling.xlsx
+++ b/keeling/OLR/OLR_keeling.xlsx
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="780">
   <si>
     <t>text</t>
   </si>
@@ -2063,9 +2063,6 @@
     <t>19.5, -155.6</t>
   </si>
   <si>
-    <t>Mauna Loa | Hawaii</t>
-  </si>
-  <si>
     <t>Keeling Curve | Atmosphere | Carbon dioxide</t>
   </si>
   <si>
@@ -2111,33 +2108,9 @@
     <t>013</t>
   </si>
   <si>
-    <t>Alert | Northwest Territory | Canada</t>
-  </si>
-  <si>
-    <t>Point Barrow | Alaska</t>
-  </si>
-  <si>
-    <t>La Jolla | California</t>
-  </si>
-  <si>
-    <t>Baja California Sur | Mexico</t>
-  </si>
-  <si>
-    <t>Cape Kumukahi | Hawaii</t>
-  </si>
-  <si>
     <t>Samoa</t>
   </si>
   <si>
-    <t>Baring Head | New Zealand</t>
-  </si>
-  <si>
-    <t>Palmer Station | Antarctica</t>
-  </si>
-  <si>
-    <t>South Pole | Antarctica</t>
-  </si>
-  <si>
     <t>82.3, -62.3</t>
   </si>
   <si>
@@ -2169,12 +2142,6 @@
   </si>
   <si>
     <t>-41.4, 174.9</t>
-  </si>
-  <si>
-    <t>Christmas Island | Fanning Island</t>
-  </si>
-  <si>
-    <t>Kermadec Island | Raoul Island</t>
   </si>
   <si>
     <t>1985 - present</t>
@@ -2532,9 +2499,6 @@
     <t>Keeling, Ralph F; Keeling, Charles D (2017): Atmospheric CO2 Data - Palmer Station, Antarctica. In Scripps CO2 Program Data. UC San Diego Library Digital Collections.</t>
   </si>
   <si>
-    <t>Weather Station Papa | North Pacific</t>
-  </si>
-  <si>
     <t>Keeling, Ralph F.</t>
   </si>
   <si>
@@ -2545,6 +2509,54 @@
   </si>
   <si>
     <t>Scripps CO2 Program | Scripps Institution of Oceanography</t>
+  </si>
+  <si>
+    <t>Alert (Canada) | Northwest Territory | Canada</t>
+  </si>
+  <si>
+    <t>Point Barrow (Alaska)</t>
+  </si>
+  <si>
+    <t>La Jolla (California)</t>
+  </si>
+  <si>
+    <t>Mauna Loa (Hawaii)</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2016-01-01</t>
+  </si>
+  <si>
+    <t>Cape Kumukahi (Hawaii)</t>
+  </si>
+  <si>
+    <t>Christmas Island (Kiribati) | Fanning Island (Kiribati)</t>
+  </si>
+  <si>
+    <t>Kermadec Islands | Raoul Island (Kermadec Islands)</t>
+  </si>
+  <si>
+    <t>Baring Head (New Zealand)</t>
+  </si>
+  <si>
+    <t>South Pole (Antarctica)</t>
+  </si>
+  <si>
+    <t>Keeling Curve | Atmosphere | Carbon dioxide | Weather Station Papa</t>
+  </si>
+  <si>
+    <t>North Pacific Ocean</t>
+  </si>
+  <si>
+    <t>Baja California Sur (Mexico)</t>
+  </si>
+  <si>
+    <t>Palmer Station</t>
+  </si>
+  <si>
+    <t>Antarctica</t>
   </si>
 </sst>
 </file>
@@ -3655,11 +3667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,20 +3687,22 @@
     <col min="9" max="9" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="27.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="3" customWidth="1"/>
     <col min="13" max="13" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="64.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" style="23" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="63" style="3" customWidth="1"/>
-    <col min="20" max="20" width="42.85546875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="70.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14" style="3" customWidth="1"/>
+    <col min="15" max="16" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.7109375" style="23" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="63" style="3" customWidth="1"/>
+    <col min="21" max="21" width="42.85546875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="70.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3729,45 +3743,51 @@
         <v>489</v>
       </c>
       <c r="N1" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>506</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>455</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>403</v>
@@ -3779,66 +3799,66 @@
         <v>361</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>694</v>
+        <v>683</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>679</v>
+        <v>658</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>721</v>
-      </c>
-      <c r="Q2" s="24" t="s">
-        <v>734</v>
+        <v>668</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>710</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>758</v>
-      </c>
-      <c r="T2" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>632</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>633</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>403</v>
@@ -3850,66 +3870,66 @@
         <v>361</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>695</v>
+        <v>684</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>670</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>680</v>
+        <v>659</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="Q3" s="24" t="s">
-        <v>734</v>
+        <v>666</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>711</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>759</v>
+        <v>723</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>632</v>
+        <v>748</v>
       </c>
       <c r="U3" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="Y3" s="3" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>710</v>
+        <v>699</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>403</v>
@@ -3921,66 +3941,66 @@
         <v>361</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>682</v>
+        <v>634</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="P4" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="R4" s="24" t="s">
         <v>723</v>
       </c>
-      <c r="Q4" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>760</v>
+      <c r="S4" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>632</v>
+        <v>749</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>649</v>
+        <v>631</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+        <v>766</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>403</v>
@@ -3992,66 +4012,66 @@
         <v>361</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>678</v>
-      </c>
       <c r="O5" s="3" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>734</v>
+        <v>666</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>713</v>
       </c>
       <c r="R5" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>761</v>
+        <v>723</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>632</v>
+        <v>750</v>
       </c>
       <c r="U5" s="3" t="s">
         <v>631</v>
       </c>
       <c r="V5" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="W5" s="3" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="Y5" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>709</v>
+        <v>698</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>403</v>
@@ -4063,66 +4083,66 @@
         <v>361</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>700</v>
+        <v>689</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M6" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>725</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>734</v>
+      <c r="P6" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>714</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>762</v>
+        <v>723</v>
+      </c>
+      <c r="S6" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>632</v>
+        <v>751</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+        <v>770</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>403</v>
@@ -4134,66 +4154,66 @@
         <v>361</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M7" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>677</v>
-      </c>
       <c r="P7" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="Q7" s="24" t="s">
-        <v>734</v>
+        <v>666</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>715</v>
       </c>
       <c r="R7" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>763</v>
+        <v>723</v>
+      </c>
+      <c r="S7" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>632</v>
+        <v>752</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>667</v>
+        <v>631</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+        <v>771</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>403</v>
@@ -4205,66 +4225,66 @@
         <v>361</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M8" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>728</v>
-      </c>
-      <c r="Q8" s="24" t="s">
-        <v>734</v>
+      <c r="P8" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>717</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>764</v>
+        <v>723</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>632</v>
+        <v>753</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>652</v>
+        <v>631</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>403</v>
@@ -4276,66 +4296,66 @@
         <v>361</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>761</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>762</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="R9" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="V9" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>773</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>774</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>718</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="Q9" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="R9" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="X9" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>712</v>
+        <v>701</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>403</v>
@@ -4347,66 +4367,66 @@
         <v>361</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>702</v>
+        <v>691</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>688</v>
+        <v>665</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="P10" s="22" t="s">
+      <c r="P10" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>721</v>
+      </c>
+      <c r="R10" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="S10" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="Y10" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="Q10" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>403</v>
@@ -4418,66 +4438,66 @@
         <v>361</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J11" s="23" t="s">
+        <v>762</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>720</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="V11" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>718</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="P11" s="22" t="s">
-        <v>731</v>
-      </c>
-      <c r="Q11" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="R11" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="X11" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>717</v>
+        <v>706</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>403</v>
@@ -4489,66 +4509,67 @@
         <v>361</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>696</v>
+        <v>685</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K12" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>737</v>
+      </c>
+      <c r="R12" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="S12" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="U12" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="L12" s="23" t="s">
-        <v>718</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>748</v>
-      </c>
-      <c r="Q12" s="24" t="s">
-        <v>733</v>
-      </c>
-      <c r="R12" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="U12" s="23" t="s">
-        <v>771</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="V12" s="23" t="s">
+        <v>776</v>
+      </c>
+      <c r="W12" s="23"/>
+      <c r="X12" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>403</v>
@@ -4560,66 +4581,66 @@
         <v>361</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M13" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>749</v>
-      </c>
-      <c r="Q13" s="24" t="s">
-        <v>733</v>
+      <c r="P13" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>738</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>769</v>
+        <v>722</v>
+      </c>
+      <c r="S13" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>632</v>
+        <v>758</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>650</v>
+        <v>631</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+        <v>777</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>713</v>
+        <v>702</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>403</v>
@@ -4631,91 +4652,112 @@
         <v>361</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>720</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>689</v>
+        <v>709</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>690</v>
+        <v>678</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>750</v>
-      </c>
-      <c r="Q14" s="24" t="s">
-        <v>733</v>
+        <v>679</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>739</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>770</v>
+        <v>722</v>
+      </c>
+      <c r="S14" s="24" t="s">
+        <v>746</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>632</v>
+        <v>759</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>654</v>
+        <v>631</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>665</v>
+        <v>779</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+        <v>778</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>753</v>
+        <v>742</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>361</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
       <c r="L15" s="23"/>
+      <c r="N15" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>769</v>
+      </c>
       <c r="P15" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>756</v>
+        <v>666</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -4741,7 +4783,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -4752,25 +4794,25 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:M1</xm:sqref>
+          <xm:sqref>L1:N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>T1:U1</xm:sqref>
+          <xm:sqref>U1:W1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
           </x14:formula1>
-          <xm:sqref>V1</xm:sqref>
+          <xm:sqref>X1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>W1</xm:sqref>
+          <xm:sqref>Y1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
@@ -4788,19 +4830,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:S1</xm:sqref>
+          <xm:sqref>Q1:T1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'[1]Select-a-header values'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:J1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'[1]Select-a-header values'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>K1</xm:sqref>
+          <xm:sqref>H1:K1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>